<commit_message>
Jane Last Update on Leave Card 1/30/2024 4:26 pm
</commit_message>
<xml_diff>
--- a/REGULAR/CCT/BANICO, PILAR.xlsx
+++ b/REGULAR/CCT/BANICO, PILAR.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="306">
   <si>
     <t>PERIOD</t>
   </si>
@@ -1047,6 +1047,30 @@
   </si>
   <si>
     <t>12/27-29/2023</t>
+  </si>
+  <si>
+    <t>2024</t>
+  </si>
+  <si>
+    <t>A(2-0-0)</t>
+  </si>
+  <si>
+    <t>11/10,13/2023</t>
+  </si>
+  <si>
+    <t>UT(0-0-52)</t>
+  </si>
+  <si>
+    <t>A(1-0-0)</t>
+  </si>
+  <si>
+    <t>UT(0-0-9)</t>
+  </si>
+  <si>
+    <t>A(3-0-0)</t>
+  </si>
+  <si>
+    <t>3/9,10,13/2023</t>
   </si>
 </sst>
 </file>
@@ -1750,7 +1774,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A8:K523" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A8:K531" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
   <tableColumns count="11">
     <tableColumn id="1" name="PERIOD" dataDxfId="10"/>
     <tableColumn id="2" name="PARTICULARS" dataDxfId="9"/>
@@ -2079,12 +2103,12 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:M523"/>
+  <dimension ref="A2:M531"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3690" topLeftCell="A385" activePane="bottomLeft"/>
+      <pane ySplit="3690" topLeftCell="A391" activePane="bottomLeft"/>
       <selection activeCell="M9" sqref="M9"/>
-      <selection pane="bottomLeft" activeCell="E406" sqref="E406"/>
+      <selection pane="bottomLeft" activeCell="E399" sqref="E399"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2249,7 +2273,7 @@
       <c r="D9" s="11"/>
       <c r="E9" s="13">
         <f>SUM(Table1[EARNED])-SUM(Table1[Absence Undertime W/ Pay])+CONVERTION!$A$3</f>
-        <v>177.71599999999998</v>
+        <v>172.77399999999997</v>
       </c>
       <c r="F9" s="11"/>
       <c r="G9" s="13" t="str">
@@ -2259,7 +2283,7 @@
       <c r="H9" s="11"/>
       <c r="I9" s="13">
         <f>SUM(Table1[[EARNED ]])-SUM(Table1[Absence Undertime  W/ Pay])+CONVERTION!$B$3</f>
-        <v>245.05599999999998</v>
+        <v>246.30599999999998</v>
       </c>
       <c r="J9" s="11"/>
       <c r="K9" s="20"/>
@@ -10544,43 +10568,41 @@
       </c>
     </row>
     <row r="395" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A395" s="40">
-        <v>44986</v>
-      </c>
+      <c r="A395" s="40"/>
       <c r="B395" s="20" t="s">
-        <v>116</v>
-      </c>
-      <c r="C395" s="13">
-        <v>1.25</v>
-      </c>
-      <c r="D395" s="39"/>
+        <v>56</v>
+      </c>
+      <c r="C395" s="13"/>
+      <c r="D395" s="39">
+        <v>8.0000000000000002E-3</v>
+      </c>
       <c r="E395" s="9"/>
       <c r="F395" s="20"/>
-      <c r="G395" s="13">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v>1.25</v>
-      </c>
-      <c r="H395" s="39">
-        <v>1</v>
-      </c>
+      <c r="G395" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H395" s="39"/>
       <c r="I395" s="9"/>
       <c r="J395" s="11"/>
-      <c r="K395" s="49">
-        <v>45012</v>
-      </c>
+      <c r="K395" s="49"/>
     </row>
     <row r="396" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A396" s="40"/>
+      <c r="A396" s="40">
+        <v>44986</v>
+      </c>
       <c r="B396" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="C396" s="13"/>
+      <c r="C396" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D396" s="39"/>
       <c r="E396" s="9"/>
       <c r="F396" s="20"/>
-      <c r="G396" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G396" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H396" s="39">
         <v>1</v>
@@ -10588,25 +10610,21 @@
       <c r="I396" s="9"/>
       <c r="J396" s="11"/>
       <c r="K396" s="49">
-        <v>44999</v>
+        <v>45012</v>
       </c>
     </row>
     <row r="397" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A397" s="40">
-        <v>45017</v>
-      </c>
+      <c r="A397" s="40"/>
       <c r="B397" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="C397" s="13">
-        <v>1.25</v>
-      </c>
+      <c r="C397" s="13"/>
       <c r="D397" s="39"/>
       <c r="E397" s="9"/>
       <c r="F397" s="20"/>
-      <c r="G397" s="13">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v>1.25</v>
+      <c r="G397" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
       </c>
       <c r="H397" s="39">
         <v>1</v>
@@ -10614,61 +10632,63 @@
       <c r="I397" s="9"/>
       <c r="J397" s="11"/>
       <c r="K397" s="49">
-        <v>45036</v>
+        <v>44999</v>
       </c>
     </row>
     <row r="398" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A398" s="40">
-        <v>45047</v>
-      </c>
+      <c r="A398" s="40"/>
       <c r="B398" s="20" t="s">
-        <v>107</v>
-      </c>
-      <c r="C398" s="13">
-        <v>1.25</v>
-      </c>
-      <c r="D398" s="39"/>
+        <v>304</v>
+      </c>
+      <c r="C398" s="13"/>
+      <c r="D398" s="39">
+        <v>3</v>
+      </c>
       <c r="E398" s="9"/>
       <c r="F398" s="20"/>
-      <c r="G398" s="13">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v>1.25</v>
+      <c r="G398" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
       </c>
       <c r="H398" s="39"/>
       <c r="I398" s="9"/>
       <c r="J398" s="11"/>
-      <c r="K398" s="49">
-        <v>45075</v>
+      <c r="K398" s="49" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="399" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A399" s="40"/>
+      <c r="A399" s="40">
+        <v>45017</v>
+      </c>
       <c r="B399" s="20" t="s">
-        <v>128</v>
-      </c>
-      <c r="C399" s="13"/>
-      <c r="D399" s="39">
-        <v>5</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="C399" s="13">
+        <v>1.25</v>
+      </c>
+      <c r="D399" s="39"/>
       <c r="E399" s="9"/>
       <c r="F399" s="20"/>
-      <c r="G399" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
-      </c>
-      <c r="H399" s="39"/>
+      <c r="G399" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
+      </c>
+      <c r="H399" s="39">
+        <v>1</v>
+      </c>
       <c r="I399" s="9"/>
       <c r="J399" s="11"/>
-      <c r="K399" s="49" t="s">
-        <v>290</v>
+      <c r="K399" s="49">
+        <v>45036</v>
       </c>
     </row>
     <row r="400" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A400" s="40">
-        <v>45078</v>
+        <v>45047</v>
       </c>
       <c r="B400" s="20" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="C400" s="13">
         <v>1.25</v>
@@ -10680,46 +10700,42 @@
         <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
         <v>1.25</v>
       </c>
-      <c r="H400" s="39">
-        <v>1</v>
-      </c>
+      <c r="H400" s="39"/>
       <c r="I400" s="9"/>
       <c r="J400" s="11"/>
       <c r="K400" s="49">
-        <v>45097</v>
+        <v>45075</v>
       </c>
     </row>
     <row r="401" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A401" s="40">
-        <v>45108</v>
-      </c>
+      <c r="A401" s="40"/>
       <c r="B401" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="C401" s="13">
-        <v>1.25</v>
-      </c>
-      <c r="D401" s="39"/>
+        <v>128</v>
+      </c>
+      <c r="C401" s="13"/>
+      <c r="D401" s="39">
+        <v>5</v>
+      </c>
       <c r="E401" s="9"/>
       <c r="F401" s="20"/>
-      <c r="G401" s="13">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v>1.25</v>
-      </c>
-      <c r="H401" s="39">
-        <v>2</v>
-      </c>
+      <c r="G401" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H401" s="39"/>
       <c r="I401" s="9"/>
       <c r="J401" s="11"/>
-      <c r="K401" s="20" t="s">
-        <v>291</v>
+      <c r="K401" s="49" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="402" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A402" s="40">
-        <v>45139</v>
-      </c>
-      <c r="B402" s="20"/>
+        <v>45078</v>
+      </c>
+      <c r="B402" s="20" t="s">
+        <v>116</v>
+      </c>
       <c r="C402" s="13">
         <v>1.25</v>
       </c>
@@ -10730,63 +10746,63 @@
         <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
         <v>1.25</v>
       </c>
-      <c r="H402" s="39"/>
+      <c r="H402" s="39">
+        <v>1</v>
+      </c>
       <c r="I402" s="9"/>
       <c r="J402" s="11"/>
-      <c r="K402" s="20"/>
+      <c r="K402" s="49">
+        <v>45097</v>
+      </c>
     </row>
     <row r="403" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A403" s="40">
-        <v>45170</v>
-      </c>
-      <c r="B403" s="20"/>
-      <c r="C403" s="13">
-        <v>1.25</v>
-      </c>
-      <c r="D403" s="39"/>
+      <c r="A403" s="40"/>
+      <c r="B403" s="20" t="s">
+        <v>302</v>
+      </c>
+      <c r="C403" s="13"/>
+      <c r="D403" s="39">
+        <v>1</v>
+      </c>
       <c r="E403" s="9"/>
       <c r="F403" s="20"/>
-      <c r="G403" s="13">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v>1.25</v>
+      <c r="G403" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
       </c>
       <c r="H403" s="39"/>
       <c r="I403" s="9"/>
       <c r="J403" s="11"/>
-      <c r="K403" s="20"/>
+      <c r="K403" s="49">
+        <v>45096</v>
+      </c>
     </row>
     <row r="404" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A404" s="40">
-        <v>45200</v>
-      </c>
+      <c r="A404" s="40"/>
       <c r="B404" s="20" t="s">
-        <v>116</v>
-      </c>
-      <c r="C404" s="13">
-        <v>1.25</v>
-      </c>
-      <c r="D404" s="39"/>
+        <v>303</v>
+      </c>
+      <c r="C404" s="13"/>
+      <c r="D404" s="39">
+        <v>1.9000000000000003E-2</v>
+      </c>
       <c r="E404" s="9"/>
       <c r="F404" s="20"/>
-      <c r="G404" s="13">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v>1.25</v>
-      </c>
-      <c r="H404" s="39">
-        <v>1</v>
-      </c>
+      <c r="G404" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H404" s="39"/>
       <c r="I404" s="9"/>
       <c r="J404" s="11"/>
-      <c r="K404" s="49">
-        <v>45212</v>
-      </c>
+      <c r="K404" s="49"/>
     </row>
     <row r="405" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A405" s="40">
-        <v>45231</v>
+        <v>45108</v>
       </c>
       <c r="B405" s="20" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="C405" s="13">
         <v>1.25</v>
@@ -10799,45 +10815,52 @@
         <v>1.25</v>
       </c>
       <c r="H405" s="39">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I405" s="9"/>
       <c r="J405" s="11"/>
-      <c r="K405" s="49">
-        <v>45250</v>
+      <c r="K405" s="20" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="406" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A406" s="40"/>
-      <c r="B406" s="20" t="s">
-        <v>296</v>
-      </c>
-      <c r="C406" s="13"/>
-      <c r="D406" s="39">
-        <v>3</v>
-      </c>
+      <c r="A406" s="40">
+        <v>45139</v>
+      </c>
+      <c r="B406" s="20"/>
+      <c r="C406" s="13">
+        <v>1.25</v>
+      </c>
+      <c r="D406" s="39"/>
       <c r="E406" s="9"/>
       <c r="F406" s="20"/>
-      <c r="G406" s="13"/>
+      <c r="G406" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
+      </c>
       <c r="H406" s="39"/>
       <c r="I406" s="9"/>
       <c r="J406" s="11"/>
-      <c r="K406" s="49" t="s">
-        <v>297</v>
-      </c>
+      <c r="K406" s="20"/>
     </row>
     <row r="407" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A407" s="40">
-        <v>45261</v>
-      </c>
-      <c r="B407" s="20"/>
-      <c r="C407" s="13"/>
-      <c r="D407" s="39"/>
+        <v>45170</v>
+      </c>
+      <c r="B407" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="C407" s="13">
+        <v>1.25</v>
+      </c>
+      <c r="D407" s="39">
+        <v>1.7000000000000001E-2</v>
+      </c>
       <c r="E407" s="9"/>
       <c r="F407" s="20"/>
-      <c r="G407" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G407" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H407" s="39"/>
       <c r="I407" s="9"/>
@@ -10846,29 +10869,39 @@
     </row>
     <row r="408" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A408" s="40">
-        <v>45292</v>
-      </c>
-      <c r="B408" s="20"/>
-      <c r="C408" s="13"/>
+        <v>45200</v>
+      </c>
+      <c r="B408" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="C408" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D408" s="39"/>
       <c r="E408" s="9"/>
       <c r="F408" s="20"/>
-      <c r="G408" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
-      </c>
-      <c r="H408" s="39"/>
+      <c r="G408" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
+      </c>
+      <c r="H408" s="39">
+        <v>1</v>
+      </c>
       <c r="I408" s="9"/>
       <c r="J408" s="11"/>
-      <c r="K408" s="20"/>
+      <c r="K408" s="49">
+        <v>45212</v>
+      </c>
     </row>
     <row r="409" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A409" s="40">
-        <v>45323</v>
-      </c>
-      <c r="B409" s="20"/>
+      <c r="A409" s="40"/>
+      <c r="B409" s="20" t="s">
+        <v>301</v>
+      </c>
       <c r="C409" s="13"/>
-      <c r="D409" s="39"/>
+      <c r="D409" s="39">
+        <v>0.10800000000000001</v>
+      </c>
       <c r="E409" s="9"/>
       <c r="F409" s="20"/>
       <c r="G409" s="13" t="str">
@@ -10878,51 +10911,62 @@
       <c r="H409" s="39"/>
       <c r="I409" s="9"/>
       <c r="J409" s="11"/>
-      <c r="K409" s="20"/>
+      <c r="K409" s="49"/>
     </row>
     <row r="410" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A410" s="40">
-        <v>45352</v>
-      </c>
-      <c r="B410" s="20"/>
-      <c r="C410" s="13"/>
+        <v>45231</v>
+      </c>
+      <c r="B410" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="C410" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D410" s="39"/>
       <c r="E410" s="9"/>
       <c r="F410" s="20"/>
-      <c r="G410" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
-      </c>
-      <c r="H410" s="39"/>
+      <c r="G410" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
+      </c>
+      <c r="H410" s="39">
+        <v>1</v>
+      </c>
       <c r="I410" s="9"/>
       <c r="J410" s="11"/>
-      <c r="K410" s="20"/>
+      <c r="K410" s="49">
+        <v>45250</v>
+      </c>
     </row>
     <row r="411" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A411" s="40">
-        <v>45383</v>
-      </c>
-      <c r="B411" s="20"/>
+      <c r="A411" s="40"/>
+      <c r="B411" s="20" t="s">
+        <v>296</v>
+      </c>
       <c r="C411" s="13"/>
-      <c r="D411" s="39"/>
+      <c r="D411" s="39">
+        <v>3</v>
+      </c>
       <c r="E411" s="9"/>
       <c r="F411" s="20"/>
-      <c r="G411" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
-      </c>
+      <c r="G411" s="13"/>
       <c r="H411" s="39"/>
       <c r="I411" s="9"/>
       <c r="J411" s="11"/>
-      <c r="K411" s="20"/>
+      <c r="K411" s="49" t="s">
+        <v>297</v>
+      </c>
     </row>
     <row r="412" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A412" s="40">
-        <v>45413</v>
-      </c>
-      <c r="B412" s="20"/>
+      <c r="A412" s="40"/>
+      <c r="B412" s="20" t="s">
+        <v>299</v>
+      </c>
       <c r="C412" s="13"/>
-      <c r="D412" s="39"/>
+      <c r="D412" s="39">
+        <v>2</v>
+      </c>
       <c r="E412" s="9"/>
       <c r="F412" s="20"/>
       <c r="G412" s="13" t="str">
@@ -10932,15 +10976,19 @@
       <c r="H412" s="39"/>
       <c r="I412" s="9"/>
       <c r="J412" s="11"/>
-      <c r="K412" s="20"/>
+      <c r="K412" s="49" t="s">
+        <v>300</v>
+      </c>
     </row>
     <row r="413" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A413" s="40">
-        <v>45444</v>
-      </c>
-      <c r="B413" s="20"/>
+      <c r="A413" s="40"/>
+      <c r="B413" s="20" t="s">
+        <v>62</v>
+      </c>
       <c r="C413" s="13"/>
-      <c r="D413" s="39"/>
+      <c r="D413" s="39">
+        <v>0.04</v>
+      </c>
       <c r="E413" s="9"/>
       <c r="F413" s="20"/>
       <c r="G413" s="13" t="str">
@@ -10950,20 +10998,22 @@
       <c r="H413" s="39"/>
       <c r="I413" s="9"/>
       <c r="J413" s="11"/>
-      <c r="K413" s="20"/>
+      <c r="K413" s="49"/>
     </row>
     <row r="414" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A414" s="40">
-        <v>45474</v>
+        <v>45261</v>
       </c>
       <c r="B414" s="20"/>
-      <c r="C414" s="13"/>
+      <c r="C414" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D414" s="39"/>
       <c r="E414" s="9"/>
       <c r="F414" s="20"/>
-      <c r="G414" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G414" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H414" s="39"/>
       <c r="I414" s="9"/>
@@ -10971,8 +11021,8 @@
       <c r="K414" s="20"/>
     </row>
     <row r="415" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A415" s="40">
-        <v>45505</v>
+      <c r="A415" s="48" t="s">
+        <v>298</v>
       </c>
       <c r="B415" s="20"/>
       <c r="C415" s="13"/>
@@ -10990,7 +11040,7 @@
     </row>
     <row r="416" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A416" s="40">
-        <v>45536</v>
+        <v>45292</v>
       </c>
       <c r="B416" s="20"/>
       <c r="C416" s="13"/>
@@ -11008,7 +11058,7 @@
     </row>
     <row r="417" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A417" s="40">
-        <v>45566</v>
+        <v>45323</v>
       </c>
       <c r="B417" s="20"/>
       <c r="C417" s="13"/>
@@ -11026,7 +11076,7 @@
     </row>
     <row r="418" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A418" s="40">
-        <v>45597</v>
+        <v>45352</v>
       </c>
       <c r="B418" s="20"/>
       <c r="C418" s="13"/>
@@ -11044,7 +11094,7 @@
     </row>
     <row r="419" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A419" s="40">
-        <v>45627</v>
+        <v>45383</v>
       </c>
       <c r="B419" s="20"/>
       <c r="C419" s="13"/>
@@ -11062,7 +11112,7 @@
     </row>
     <row r="420" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A420" s="40">
-        <v>45658</v>
+        <v>45413</v>
       </c>
       <c r="B420" s="20"/>
       <c r="C420" s="13"/>
@@ -11080,7 +11130,7 @@
     </row>
     <row r="421" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A421" s="40">
-        <v>45689</v>
+        <v>45444</v>
       </c>
       <c r="B421" s="20"/>
       <c r="C421" s="13"/>
@@ -11098,7 +11148,7 @@
     </row>
     <row r="422" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A422" s="40">
-        <v>45717</v>
+        <v>45474</v>
       </c>
       <c r="B422" s="20"/>
       <c r="C422" s="13"/>
@@ -11116,7 +11166,7 @@
     </row>
     <row r="423" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A423" s="40">
-        <v>45748</v>
+        <v>45505</v>
       </c>
       <c r="B423" s="20"/>
       <c r="C423" s="13"/>
@@ -11134,7 +11184,7 @@
     </row>
     <row r="424" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A424" s="40">
-        <v>45778</v>
+        <v>45536</v>
       </c>
       <c r="B424" s="20"/>
       <c r="C424" s="13"/>
@@ -11152,7 +11202,7 @@
     </row>
     <row r="425" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A425" s="40">
-        <v>45809</v>
+        <v>45566</v>
       </c>
       <c r="B425" s="20"/>
       <c r="C425" s="13"/>
@@ -11170,7 +11220,7 @@
     </row>
     <row r="426" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A426" s="40">
-        <v>45839</v>
+        <v>45597</v>
       </c>
       <c r="B426" s="20"/>
       <c r="C426" s="13"/>
@@ -11188,7 +11238,7 @@
     </row>
     <row r="427" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A427" s="40">
-        <v>45870</v>
+        <v>45627</v>
       </c>
       <c r="B427" s="20"/>
       <c r="C427" s="13"/>
@@ -11206,7 +11256,7 @@
     </row>
     <row r="428" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A428" s="40">
-        <v>45901</v>
+        <v>45658</v>
       </c>
       <c r="B428" s="20"/>
       <c r="C428" s="13"/>
@@ -11224,7 +11274,7 @@
     </row>
     <row r="429" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A429" s="40">
-        <v>45931</v>
+        <v>45689</v>
       </c>
       <c r="B429" s="20"/>
       <c r="C429" s="13"/>
@@ -11242,7 +11292,7 @@
     </row>
     <row r="430" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A430" s="40">
-        <v>45962</v>
+        <v>45717</v>
       </c>
       <c r="B430" s="20"/>
       <c r="C430" s="13"/>
@@ -11260,7 +11310,7 @@
     </row>
     <row r="431" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A431" s="40">
-        <v>45992</v>
+        <v>45748</v>
       </c>
       <c r="B431" s="20"/>
       <c r="C431" s="13"/>
@@ -11278,7 +11328,7 @@
     </row>
     <row r="432" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A432" s="40">
-        <v>46023</v>
+        <v>45778</v>
       </c>
       <c r="B432" s="20"/>
       <c r="C432" s="13"/>
@@ -11296,7 +11346,7 @@
     </row>
     <row r="433" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A433" s="40">
-        <v>46054</v>
+        <v>45809</v>
       </c>
       <c r="B433" s="20"/>
       <c r="C433" s="13"/>
@@ -11314,7 +11364,7 @@
     </row>
     <row r="434" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A434" s="40">
-        <v>46082</v>
+        <v>45839</v>
       </c>
       <c r="B434" s="20"/>
       <c r="C434" s="13"/>
@@ -11332,7 +11382,7 @@
     </row>
     <row r="435" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A435" s="40">
-        <v>46113</v>
+        <v>45870</v>
       </c>
       <c r="B435" s="20"/>
       <c r="C435" s="13"/>
@@ -11350,7 +11400,7 @@
     </row>
     <row r="436" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A436" s="40">
-        <v>46143</v>
+        <v>45901</v>
       </c>
       <c r="B436" s="20"/>
       <c r="C436" s="13"/>
@@ -11368,7 +11418,7 @@
     </row>
     <row r="437" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A437" s="40">
-        <v>46174</v>
+        <v>45931</v>
       </c>
       <c r="B437" s="20"/>
       <c r="C437" s="13"/>
@@ -11386,7 +11436,7 @@
     </row>
     <row r="438" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A438" s="40">
-        <v>46204</v>
+        <v>45962</v>
       </c>
       <c r="B438" s="20"/>
       <c r="C438" s="13"/>
@@ -11404,7 +11454,7 @@
     </row>
     <row r="439" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A439" s="40">
-        <v>46235</v>
+        <v>45992</v>
       </c>
       <c r="B439" s="20"/>
       <c r="C439" s="13"/>
@@ -11422,7 +11472,7 @@
     </row>
     <row r="440" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A440" s="40">
-        <v>46266</v>
+        <v>46023</v>
       </c>
       <c r="B440" s="20"/>
       <c r="C440" s="13"/>
@@ -11440,7 +11490,7 @@
     </row>
     <row r="441" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A441" s="40">
-        <v>46296</v>
+        <v>46054</v>
       </c>
       <c r="B441" s="20"/>
       <c r="C441" s="13"/>
@@ -11458,7 +11508,7 @@
     </row>
     <row r="442" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A442" s="40">
-        <v>46327</v>
+        <v>46082</v>
       </c>
       <c r="B442" s="20"/>
       <c r="C442" s="13"/>
@@ -11476,7 +11526,7 @@
     </row>
     <row r="443" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A443" s="40">
-        <v>46357</v>
+        <v>46113</v>
       </c>
       <c r="B443" s="20"/>
       <c r="C443" s="13"/>
@@ -11494,7 +11544,7 @@
     </row>
     <row r="444" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A444" s="40">
-        <v>46388</v>
+        <v>46143</v>
       </c>
       <c r="B444" s="20"/>
       <c r="C444" s="13"/>
@@ -11512,7 +11562,7 @@
     </row>
     <row r="445" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A445" s="40">
-        <v>46419</v>
+        <v>46174</v>
       </c>
       <c r="B445" s="20"/>
       <c r="C445" s="13"/>
@@ -11530,7 +11580,7 @@
     </row>
     <row r="446" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A446" s="40">
-        <v>46447</v>
+        <v>46204</v>
       </c>
       <c r="B446" s="20"/>
       <c r="C446" s="13"/>
@@ -11548,7 +11598,7 @@
     </row>
     <row r="447" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A447" s="40">
-        <v>46478</v>
+        <v>46235</v>
       </c>
       <c r="B447" s="20"/>
       <c r="C447" s="13"/>
@@ -11566,7 +11616,7 @@
     </row>
     <row r="448" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A448" s="40">
-        <v>46508</v>
+        <v>46266</v>
       </c>
       <c r="B448" s="20"/>
       <c r="C448" s="13"/>
@@ -11584,7 +11634,7 @@
     </row>
     <row r="449" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A449" s="40">
-        <v>46539</v>
+        <v>46296</v>
       </c>
       <c r="B449" s="20"/>
       <c r="C449" s="13"/>
@@ -11602,7 +11652,7 @@
     </row>
     <row r="450" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A450" s="40">
-        <v>46569</v>
+        <v>46327</v>
       </c>
       <c r="B450" s="20"/>
       <c r="C450" s="13"/>
@@ -11620,7 +11670,7 @@
     </row>
     <row r="451" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A451" s="40">
-        <v>46600</v>
+        <v>46357</v>
       </c>
       <c r="B451" s="20"/>
       <c r="C451" s="13"/>
@@ -11638,7 +11688,7 @@
     </row>
     <row r="452" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A452" s="40">
-        <v>46631</v>
+        <v>46388</v>
       </c>
       <c r="B452" s="20"/>
       <c r="C452" s="13"/>
@@ -11656,7 +11706,7 @@
     </row>
     <row r="453" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A453" s="40">
-        <v>46661</v>
+        <v>46419</v>
       </c>
       <c r="B453" s="20"/>
       <c r="C453" s="13"/>
@@ -11674,7 +11724,7 @@
     </row>
     <row r="454" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A454" s="40">
-        <v>46692</v>
+        <v>46447</v>
       </c>
       <c r="B454" s="20"/>
       <c r="C454" s="13"/>
@@ -11692,7 +11742,7 @@
     </row>
     <row r="455" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A455" s="40">
-        <v>46722</v>
+        <v>46478</v>
       </c>
       <c r="B455" s="20"/>
       <c r="C455" s="13"/>
@@ -11710,7 +11760,7 @@
     </row>
     <row r="456" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A456" s="40">
-        <v>46753</v>
+        <v>46508</v>
       </c>
       <c r="B456" s="20"/>
       <c r="C456" s="13"/>
@@ -11728,7 +11778,7 @@
     </row>
     <row r="457" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A457" s="40">
-        <v>46784</v>
+        <v>46539</v>
       </c>
       <c r="B457" s="20"/>
       <c r="C457" s="13"/>
@@ -11746,7 +11796,7 @@
     </row>
     <row r="458" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A458" s="40">
-        <v>46813</v>
+        <v>46569</v>
       </c>
       <c r="B458" s="20"/>
       <c r="C458" s="13"/>
@@ -11764,7 +11814,7 @@
     </row>
     <row r="459" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A459" s="40">
-        <v>46844</v>
+        <v>46600</v>
       </c>
       <c r="B459" s="20"/>
       <c r="C459" s="13"/>
@@ -11782,7 +11832,7 @@
     </row>
     <row r="460" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A460" s="40">
-        <v>46874</v>
+        <v>46631</v>
       </c>
       <c r="B460" s="20"/>
       <c r="C460" s="13"/>
@@ -11800,7 +11850,7 @@
     </row>
     <row r="461" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A461" s="40">
-        <v>46905</v>
+        <v>46661</v>
       </c>
       <c r="B461" s="20"/>
       <c r="C461" s="13"/>
@@ -11818,7 +11868,7 @@
     </row>
     <row r="462" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A462" s="40">
-        <v>46935</v>
+        <v>46692</v>
       </c>
       <c r="B462" s="20"/>
       <c r="C462" s="13"/>
@@ -11836,7 +11886,7 @@
     </row>
     <row r="463" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A463" s="40">
-        <v>46966</v>
+        <v>46722</v>
       </c>
       <c r="B463" s="20"/>
       <c r="C463" s="13"/>
@@ -11854,7 +11904,7 @@
     </row>
     <row r="464" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A464" s="40">
-        <v>46997</v>
+        <v>46753</v>
       </c>
       <c r="B464" s="20"/>
       <c r="C464" s="13"/>
@@ -11872,7 +11922,7 @@
     </row>
     <row r="465" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A465" s="40">
-        <v>47027</v>
+        <v>46784</v>
       </c>
       <c r="B465" s="20"/>
       <c r="C465" s="13"/>
@@ -11890,7 +11940,7 @@
     </row>
     <row r="466" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A466" s="40">
-        <v>47058</v>
+        <v>46813</v>
       </c>
       <c r="B466" s="20"/>
       <c r="C466" s="13"/>
@@ -11908,7 +11958,7 @@
     </row>
     <row r="467" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A467" s="40">
-        <v>47088</v>
+        <v>46844</v>
       </c>
       <c r="B467" s="20"/>
       <c r="C467" s="13"/>
@@ -11926,7 +11976,7 @@
     </row>
     <row r="468" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A468" s="40">
-        <v>47119</v>
+        <v>46874</v>
       </c>
       <c r="B468" s="20"/>
       <c r="C468" s="13"/>
@@ -11944,7 +11994,7 @@
     </row>
     <row r="469" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A469" s="40">
-        <v>47150</v>
+        <v>46905</v>
       </c>
       <c r="B469" s="20"/>
       <c r="C469" s="13"/>
@@ -11962,7 +12012,7 @@
     </row>
     <row r="470" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A470" s="40">
-        <v>47178</v>
+        <v>46935</v>
       </c>
       <c r="B470" s="20"/>
       <c r="C470" s="13"/>
@@ -11980,7 +12030,7 @@
     </row>
     <row r="471" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A471" s="40">
-        <v>47209</v>
+        <v>46966</v>
       </c>
       <c r="B471" s="20"/>
       <c r="C471" s="13"/>
@@ -11998,7 +12048,7 @@
     </row>
     <row r="472" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A472" s="40">
-        <v>47239</v>
+        <v>46997</v>
       </c>
       <c r="B472" s="20"/>
       <c r="C472" s="13"/>
@@ -12016,7 +12066,7 @@
     </row>
     <row r="473" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A473" s="40">
-        <v>47270</v>
+        <v>47027</v>
       </c>
       <c r="B473" s="20"/>
       <c r="C473" s="13"/>
@@ -12034,7 +12084,7 @@
     </row>
     <row r="474" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A474" s="40">
-        <v>47300</v>
+        <v>47058</v>
       </c>
       <c r="B474" s="20"/>
       <c r="C474" s="13"/>
@@ -12052,7 +12102,7 @@
     </row>
     <row r="475" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A475" s="40">
-        <v>47331</v>
+        <v>47088</v>
       </c>
       <c r="B475" s="20"/>
       <c r="C475" s="13"/>
@@ -12070,7 +12120,7 @@
     </row>
     <row r="476" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A476" s="40">
-        <v>47362</v>
+        <v>47119</v>
       </c>
       <c r="B476" s="20"/>
       <c r="C476" s="13"/>
@@ -12088,7 +12138,7 @@
     </row>
     <row r="477" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A477" s="40">
-        <v>47392</v>
+        <v>47150</v>
       </c>
       <c r="B477" s="20"/>
       <c r="C477" s="13"/>
@@ -12106,7 +12156,7 @@
     </row>
     <row r="478" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A478" s="40">
-        <v>47423</v>
+        <v>47178</v>
       </c>
       <c r="B478" s="20"/>
       <c r="C478" s="13"/>
@@ -12124,7 +12174,7 @@
     </row>
     <row r="479" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A479" s="40">
-        <v>47453</v>
+        <v>47209</v>
       </c>
       <c r="B479" s="20"/>
       <c r="C479" s="13"/>
@@ -12142,7 +12192,7 @@
     </row>
     <row r="480" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A480" s="40">
-        <v>47484</v>
+        <v>47239</v>
       </c>
       <c r="B480" s="20"/>
       <c r="C480" s="13"/>
@@ -12160,7 +12210,7 @@
     </row>
     <row r="481" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A481" s="40">
-        <v>47515</v>
+        <v>47270</v>
       </c>
       <c r="B481" s="20"/>
       <c r="C481" s="13"/>
@@ -12178,7 +12228,7 @@
     </row>
     <row r="482" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A482" s="40">
-        <v>47543</v>
+        <v>47300</v>
       </c>
       <c r="B482" s="20"/>
       <c r="C482" s="13"/>
@@ -12196,7 +12246,7 @@
     </row>
     <row r="483" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A483" s="40">
-        <v>47574</v>
+        <v>47331</v>
       </c>
       <c r="B483" s="20"/>
       <c r="C483" s="13"/>
@@ -12214,7 +12264,7 @@
     </row>
     <row r="484" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A484" s="40">
-        <v>47604</v>
+        <v>47362</v>
       </c>
       <c r="B484" s="20"/>
       <c r="C484" s="13"/>
@@ -12232,7 +12282,7 @@
     </row>
     <row r="485" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A485" s="40">
-        <v>47635</v>
+        <v>47392</v>
       </c>
       <c r="B485" s="20"/>
       <c r="C485" s="13"/>
@@ -12250,7 +12300,7 @@
     </row>
     <row r="486" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A486" s="40">
-        <v>47665</v>
+        <v>47423</v>
       </c>
       <c r="B486" s="20"/>
       <c r="C486" s="13"/>
@@ -12268,7 +12318,7 @@
     </row>
     <row r="487" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A487" s="40">
-        <v>47696</v>
+        <v>47453</v>
       </c>
       <c r="B487" s="20"/>
       <c r="C487" s="13"/>
@@ -12286,7 +12336,7 @@
     </row>
     <row r="488" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A488" s="40">
-        <v>47727</v>
+        <v>47484</v>
       </c>
       <c r="B488" s="20"/>
       <c r="C488" s="13"/>
@@ -12304,7 +12354,7 @@
     </row>
     <row r="489" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A489" s="40">
-        <v>47757</v>
+        <v>47515</v>
       </c>
       <c r="B489" s="20"/>
       <c r="C489" s="13"/>
@@ -12322,7 +12372,7 @@
     </row>
     <row r="490" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A490" s="40">
-        <v>47788</v>
+        <v>47543</v>
       </c>
       <c r="B490" s="20"/>
       <c r="C490" s="13"/>
@@ -12340,7 +12390,7 @@
     </row>
     <row r="491" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A491" s="40">
-        <v>47818</v>
+        <v>47574</v>
       </c>
       <c r="B491" s="20"/>
       <c r="C491" s="13"/>
@@ -12358,7 +12408,7 @@
     </row>
     <row r="492" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A492" s="40">
-        <v>47849</v>
+        <v>47604</v>
       </c>
       <c r="B492" s="20"/>
       <c r="C492" s="13"/>
@@ -12376,7 +12426,7 @@
     </row>
     <row r="493" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A493" s="40">
-        <v>47880</v>
+        <v>47635</v>
       </c>
       <c r="B493" s="20"/>
       <c r="C493" s="13"/>
@@ -12394,7 +12444,7 @@
     </row>
     <row r="494" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A494" s="40">
-        <v>47908</v>
+        <v>47665</v>
       </c>
       <c r="B494" s="20"/>
       <c r="C494" s="13"/>
@@ -12412,7 +12462,7 @@
     </row>
     <row r="495" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A495" s="40">
-        <v>47939</v>
+        <v>47696</v>
       </c>
       <c r="B495" s="20"/>
       <c r="C495" s="13"/>
@@ -12430,7 +12480,7 @@
     </row>
     <row r="496" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A496" s="40">
-        <v>47969</v>
+        <v>47727</v>
       </c>
       <c r="B496" s="20"/>
       <c r="C496" s="13"/>
@@ -12448,7 +12498,7 @@
     </row>
     <row r="497" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A497" s="40">
-        <v>48000</v>
+        <v>47757</v>
       </c>
       <c r="B497" s="20"/>
       <c r="C497" s="13"/>
@@ -12466,7 +12516,7 @@
     </row>
     <row r="498" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A498" s="40">
-        <v>48030</v>
+        <v>47788</v>
       </c>
       <c r="B498" s="20"/>
       <c r="C498" s="13"/>
@@ -12484,7 +12534,7 @@
     </row>
     <row r="499" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A499" s="40">
-        <v>48061</v>
+        <v>47818</v>
       </c>
       <c r="B499" s="20"/>
       <c r="C499" s="13"/>
@@ -12502,7 +12552,7 @@
     </row>
     <row r="500" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A500" s="40">
-        <v>48092</v>
+        <v>47849</v>
       </c>
       <c r="B500" s="20"/>
       <c r="C500" s="13"/>
@@ -12520,7 +12570,7 @@
     </row>
     <row r="501" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A501" s="40">
-        <v>48122</v>
+        <v>47880</v>
       </c>
       <c r="B501" s="20"/>
       <c r="C501" s="13"/>
@@ -12538,7 +12588,7 @@
     </row>
     <row r="502" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A502" s="40">
-        <v>48153</v>
+        <v>47908</v>
       </c>
       <c r="B502" s="20"/>
       <c r="C502" s="13"/>
@@ -12556,7 +12606,7 @@
     </row>
     <row r="503" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A503" s="40">
-        <v>48183</v>
+        <v>47939</v>
       </c>
       <c r="B503" s="20"/>
       <c r="C503" s="13"/>
@@ -12574,7 +12624,7 @@
     </row>
     <row r="504" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A504" s="40">
-        <v>48214</v>
+        <v>47969</v>
       </c>
       <c r="B504" s="20"/>
       <c r="C504" s="13"/>
@@ -12592,7 +12642,7 @@
     </row>
     <row r="505" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A505" s="40">
-        <v>48245</v>
+        <v>48000</v>
       </c>
       <c r="B505" s="20"/>
       <c r="C505" s="13"/>
@@ -12610,7 +12660,7 @@
     </row>
     <row r="506" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A506" s="40">
-        <v>48274</v>
+        <v>48030</v>
       </c>
       <c r="B506" s="20"/>
       <c r="C506" s="13"/>
@@ -12628,7 +12678,7 @@
     </row>
     <row r="507" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A507" s="40">
-        <v>48305</v>
+        <v>48061</v>
       </c>
       <c r="B507" s="20"/>
       <c r="C507" s="13"/>
@@ -12646,7 +12696,7 @@
     </row>
     <row r="508" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A508" s="40">
-        <v>48335</v>
+        <v>48092</v>
       </c>
       <c r="B508" s="20"/>
       <c r="C508" s="13"/>
@@ -12664,7 +12714,7 @@
     </row>
     <row r="509" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A509" s="40">
-        <v>48366</v>
+        <v>48122</v>
       </c>
       <c r="B509" s="20"/>
       <c r="C509" s="13"/>
@@ -12682,7 +12732,7 @@
     </row>
     <row r="510" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A510" s="40">
-        <v>48396</v>
+        <v>48153</v>
       </c>
       <c r="B510" s="20"/>
       <c r="C510" s="13"/>
@@ -12700,7 +12750,7 @@
     </row>
     <row r="511" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A511" s="40">
-        <v>48427</v>
+        <v>48183</v>
       </c>
       <c r="B511" s="20"/>
       <c r="C511" s="13"/>
@@ -12718,7 +12768,7 @@
     </row>
     <row r="512" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A512" s="40">
-        <v>48458</v>
+        <v>48214</v>
       </c>
       <c r="B512" s="20"/>
       <c r="C512" s="13"/>
@@ -12736,7 +12786,7 @@
     </row>
     <row r="513" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A513" s="40">
-        <v>48488</v>
+        <v>48245</v>
       </c>
       <c r="B513" s="20"/>
       <c r="C513" s="13"/>
@@ -12754,7 +12804,7 @@
     </row>
     <row r="514" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A514" s="40">
-        <v>48519</v>
+        <v>48274</v>
       </c>
       <c r="B514" s="20"/>
       <c r="C514" s="13"/>
@@ -12772,7 +12822,7 @@
     </row>
     <row r="515" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A515" s="40">
-        <v>48549</v>
+        <v>48305</v>
       </c>
       <c r="B515" s="20"/>
       <c r="C515" s="13"/>
@@ -12790,7 +12840,7 @@
     </row>
     <row r="516" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A516" s="40">
-        <v>48580</v>
+        <v>48335</v>
       </c>
       <c r="B516" s="20"/>
       <c r="C516" s="13"/>
@@ -12808,7 +12858,7 @@
     </row>
     <row r="517" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A517" s="40">
-        <v>48611</v>
+        <v>48366</v>
       </c>
       <c r="B517" s="20"/>
       <c r="C517" s="13"/>
@@ -12825,7 +12875,9 @@
       <c r="K517" s="20"/>
     </row>
     <row r="518" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A518" s="40"/>
+      <c r="A518" s="40">
+        <v>48396</v>
+      </c>
       <c r="B518" s="20"/>
       <c r="C518" s="13"/>
       <c r="D518" s="39"/>
@@ -12841,7 +12893,9 @@
       <c r="K518" s="20"/>
     </row>
     <row r="519" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A519" s="40"/>
+      <c r="A519" s="40">
+        <v>48427</v>
+      </c>
       <c r="B519" s="20"/>
       <c r="C519" s="13"/>
       <c r="D519" s="39"/>
@@ -12857,7 +12911,9 @@
       <c r="K519" s="20"/>
     </row>
     <row r="520" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A520" s="40"/>
+      <c r="A520" s="40">
+        <v>48458</v>
+      </c>
       <c r="B520" s="20"/>
       <c r="C520" s="13"/>
       <c r="D520" s="39"/>
@@ -12873,7 +12929,9 @@
       <c r="K520" s="20"/>
     </row>
     <row r="521" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A521" s="40"/>
+      <c r="A521" s="40">
+        <v>48488</v>
+      </c>
       <c r="B521" s="20"/>
       <c r="C521" s="13"/>
       <c r="D521" s="39"/>
@@ -12889,7 +12947,9 @@
       <c r="K521" s="20"/>
     </row>
     <row r="522" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A522" s="40"/>
+      <c r="A522" s="40">
+        <v>48519</v>
+      </c>
       <c r="B522" s="20"/>
       <c r="C522" s="13"/>
       <c r="D522" s="39"/>
@@ -12905,20 +12965,154 @@
       <c r="K522" s="20"/>
     </row>
     <row r="523" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A523" s="41"/>
-      <c r="B523" s="15"/>
-      <c r="C523" s="42"/>
-      <c r="D523" s="43"/>
+      <c r="A523" s="40">
+        <v>48549</v>
+      </c>
+      <c r="B523" s="20"/>
+      <c r="C523" s="13"/>
+      <c r="D523" s="39"/>
       <c r="E523" s="9"/>
-      <c r="F523" s="15"/>
+      <c r="F523" s="20"/>
       <c r="G523" s="13" t="str">
         <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
         <v/>
       </c>
-      <c r="H523" s="43"/>
+      <c r="H523" s="39"/>
       <c r="I523" s="9"/>
-      <c r="J523" s="12"/>
-      <c r="K523" s="15"/>
+      <c r="J523" s="11"/>
+      <c r="K523" s="20"/>
+    </row>
+    <row r="524" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A524" s="40">
+        <v>48580</v>
+      </c>
+      <c r="B524" s="20"/>
+      <c r="C524" s="13"/>
+      <c r="D524" s="39"/>
+      <c r="E524" s="9"/>
+      <c r="F524" s="20"/>
+      <c r="G524" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H524" s="39"/>
+      <c r="I524" s="9"/>
+      <c r="J524" s="11"/>
+      <c r="K524" s="20"/>
+    </row>
+    <row r="525" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A525" s="40">
+        <v>48611</v>
+      </c>
+      <c r="B525" s="20"/>
+      <c r="C525" s="13"/>
+      <c r="D525" s="39"/>
+      <c r="E525" s="9"/>
+      <c r="F525" s="20"/>
+      <c r="G525" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H525" s="39"/>
+      <c r="I525" s="9"/>
+      <c r="J525" s="11"/>
+      <c r="K525" s="20"/>
+    </row>
+    <row r="526" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A526" s="40"/>
+      <c r="B526" s="20"/>
+      <c r="C526" s="13"/>
+      <c r="D526" s="39"/>
+      <c r="E526" s="9"/>
+      <c r="F526" s="20"/>
+      <c r="G526" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H526" s="39"/>
+      <c r="I526" s="9"/>
+      <c r="J526" s="11"/>
+      <c r="K526" s="20"/>
+    </row>
+    <row r="527" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A527" s="40"/>
+      <c r="B527" s="20"/>
+      <c r="C527" s="13"/>
+      <c r="D527" s="39"/>
+      <c r="E527" s="9"/>
+      <c r="F527" s="20"/>
+      <c r="G527" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H527" s="39"/>
+      <c r="I527" s="9"/>
+      <c r="J527" s="11"/>
+      <c r="K527" s="20"/>
+    </row>
+    <row r="528" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A528" s="40"/>
+      <c r="B528" s="20"/>
+      <c r="C528" s="13"/>
+      <c r="D528" s="39"/>
+      <c r="E528" s="9"/>
+      <c r="F528" s="20"/>
+      <c r="G528" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H528" s="39"/>
+      <c r="I528" s="9"/>
+      <c r="J528" s="11"/>
+      <c r="K528" s="20"/>
+    </row>
+    <row r="529" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A529" s="40"/>
+      <c r="B529" s="20"/>
+      <c r="C529" s="13"/>
+      <c r="D529" s="39"/>
+      <c r="E529" s="9"/>
+      <c r="F529" s="20"/>
+      <c r="G529" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H529" s="39"/>
+      <c r="I529" s="9"/>
+      <c r="J529" s="11"/>
+      <c r="K529" s="20"/>
+    </row>
+    <row r="530" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A530" s="40"/>
+      <c r="B530" s="20"/>
+      <c r="C530" s="13"/>
+      <c r="D530" s="39"/>
+      <c r="E530" s="9"/>
+      <c r="F530" s="20"/>
+      <c r="G530" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H530" s="39"/>
+      <c r="I530" s="9"/>
+      <c r="J530" s="11"/>
+      <c r="K530" s="20"/>
+    </row>
+    <row r="531" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A531" s="41"/>
+      <c r="B531" s="15"/>
+      <c r="C531" s="42"/>
+      <c r="D531" s="43"/>
+      <c r="E531" s="9"/>
+      <c r="F531" s="15"/>
+      <c r="G531" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H531" s="43"/>
+      <c r="I531" s="9"/>
+      <c r="J531" s="12"/>
+      <c r="K531" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -13030,11 +13224,11 @@
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="G3" s="45">
         <f>SUMIFS(F7:F14,E7:E14,E3)+SUMIFS(D7:D66,C7:C66,F3)+D3</f>
-        <v>3.3000000000000015E-2</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="J3" s="47"/>
       <c r="K3" s="35">

</xml_diff>